<commit_message>
Added u_entry to penarikan
</commit_message>
<xml_diff>
--- a/public/template-excel/template-penarikan.xlsx
+++ b/public/template-excel/template-penarikan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DBL\Project\webserver\project\simpin\public\template-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31607D1A-28E6-4D0F-9EB2-8CCA0F0D901E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D255FD-09F5-4768-84ED-3DF64F416597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>kode_anggota</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>411.01.000</t>
+  </si>
+  <si>
+    <t>u_entry</t>
   </si>
 </sst>
 </file>
@@ -886,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +905,7 @@
     <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -921,8 +924,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6067</v>
       </c>

</xml_diff>